<commit_message>
Corrected some small mistakes
</commit_message>
<xml_diff>
--- a/excel/tuner.xlsx
+++ b/excel/tuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfredo.CELPLANUS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E8BBAEB-CC71-4759-B432-088293A86AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B573A9A8-F1E6-474E-B646-0D738B72EAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5E2A74D-75EF-4F4E-9939-B924DF3501C3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="27">
   <si>
     <t>A4 Pitch</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>F Err</t>
-  </si>
-  <si>
-    <t>`</t>
   </si>
 </sst>
 </file>
@@ -553,7 +550,7 @@
   <dimension ref="A1:T111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,21 +601,21 @@
       <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" t="e">
+      <c r="Q1">
         <f>MIN(E4:E111)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R1" t="e">
+        <v>-1.3173492615260329</v>
+      </c>
+      <c r="R1">
         <f>MAX(E4:E111)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S1" t="e">
+        <v>1.3342285156377329</v>
+      </c>
+      <c r="S1">
         <f>AVERAGE(E4:E111)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T1" t="e">
+        <v>3.343558368322154E-2</v>
+      </c>
+      <c r="T1">
         <f>STDEV(E4:E111)</f>
-        <v>#VALUE!</v>
+        <v>0.79945573399802961</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -2035,16 +2032,17 @@
       <c r="B72" s="9">
         <v>5</v>
       </c>
-      <c r="C72" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D72" s="6" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E72" s="6" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+      <c r="C72" s="6">
+        <f t="shared" si="4"/>
+        <v>830.6093951598906</v>
+      </c>
+      <c r="D72" s="6">
+        <f t="shared" si="5"/>
+        <v>309</v>
+      </c>
+      <c r="E72" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.110575543234404</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2054,17 +2052,17 @@
       <c r="B73" s="9">
         <v>5</v>
       </c>
-      <c r="C73" s="6" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D73" s="6" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E73" s="6" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+      <c r="C73" s="6">
+        <f t="shared" si="4"/>
+        <v>880.00000000000034</v>
+      </c>
+      <c r="D73" s="6">
+        <f t="shared" si="5"/>
+        <v>327</v>
+      </c>
+      <c r="E73" s="6">
+        <f t="shared" si="3"/>
+        <v>-0.16967773437465894</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2074,17 +2072,17 @@
       <c r="B74" s="9">
         <v>5</v>
       </c>
-      <c r="C74" s="6" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D74" s="6" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E74" s="6" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+      <c r="C74" s="6">
+        <f t="shared" si="4"/>
+        <v>932.3275230361802</v>
+      </c>
+      <c r="D74" s="6">
+        <f t="shared" si="5"/>
+        <v>346</v>
+      </c>
+      <c r="E74" s="6">
+        <f t="shared" si="3"/>
+        <v>1.016487879930196</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2094,17 +2092,17 @@
       <c r="B75" s="9">
         <v>5</v>
       </c>
-      <c r="C75" s="6" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D75" s="6" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E75" s="6" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+      <c r="C75" s="6">
+        <f t="shared" si="4"/>
+        <v>987.7666025122486</v>
+      </c>
+      <c r="D75" s="6">
+        <f t="shared" si="5"/>
+        <v>367</v>
+      </c>
+      <c r="E75" s="6">
+        <f t="shared" si="3"/>
+        <v>-6.9090847126403787E-2</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2114,17 +2112,17 @@
       <c r="B76" s="9">
         <v>6</v>
       </c>
-      <c r="C76" s="6" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D76" s="6" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E76" s="6" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+      <c r="C76" s="6">
+        <f t="shared" si="4"/>
+        <v>1046.5022612023949</v>
+      </c>
+      <c r="D76" s="6">
+        <f t="shared" si="5"/>
+        <v>389</v>
+      </c>
+      <c r="E76" s="6">
+        <f t="shared" si="3"/>
+        <v>-0.54974075073005224</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2134,17 +2132,17 @@
       <c r="B77" s="9">
         <v>6</v>
       </c>
-      <c r="C77" s="6" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D77" s="6" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E77" s="6" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+      <c r="C77" s="6">
+        <f t="shared" si="4"/>
+        <v>1108.7305239074888</v>
+      </c>
+      <c r="D77" s="6">
+        <f t="shared" si="5"/>
+        <v>412</v>
+      </c>
+      <c r="E77" s="6">
+        <f t="shared" si="3"/>
+        <v>-0.22943703001124049</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2154,17 +2152,17 @@
       <c r="B78" s="9">
         <v>6</v>
       </c>
-      <c r="C78" s="6" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D78" s="6" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E78" s="6" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+      <c r="C78" s="6">
+        <f t="shared" si="4"/>
+        <v>1174.6590716696307</v>
+      </c>
+      <c r="D78" s="6">
+        <f t="shared" si="5"/>
+        <v>436</v>
+      </c>
+      <c r="E78" s="6">
+        <f t="shared" si="3"/>
+        <v>1.0995013571307481</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2174,17 +2172,17 @@
       <c r="B79" s="9">
         <v>6</v>
       </c>
-      <c r="C79" s="6" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D79" s="6" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E79" s="6" t="e">
+      <c r="C79" s="6">
+        <f t="shared" si="4"/>
+        <v>1244.5079348883241</v>
+      </c>
+      <c r="D79" s="6">
+        <f t="shared" si="5"/>
+        <v>462</v>
+      </c>
+      <c r="E79" s="6">
         <f t="shared" ref="E79:E111" si="6">C79-D79*$N$1</f>
-        <v>#VALUE!</v>
+        <v>0.96545441957414369</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2194,17 +2192,17 @@
       <c r="B80" s="9">
         <v>6</v>
       </c>
-      <c r="C80" s="6" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D80" s="6" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E80" s="6" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C80" s="6">
+        <f t="shared" si="4"/>
+        <v>1318.5102276514804</v>
+      </c>
+      <c r="D80" s="6">
+        <f t="shared" si="5"/>
+        <v>490</v>
+      </c>
+      <c r="E80" s="6">
+        <f t="shared" si="6"/>
+        <v>-0.39846375476963658</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2214,17 +2212,17 @@
       <c r="B81">
         <v>6</v>
       </c>
-      <c r="C81" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D81" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E81" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C81">
+        <f t="shared" si="4"/>
+        <v>1396.9129257320162</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="5"/>
+        <v>519</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="6"/>
+        <v>-5.3627002358780373E-2</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2234,17 +2232,17 @@
       <c r="B82">
         <v>6</v>
       </c>
-      <c r="C82" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D82" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E82" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C82">
+        <f t="shared" si="4"/>
+        <v>1479.9776908465383</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="5"/>
+        <v>550</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="6"/>
+        <v>-0.43002399721171969</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2254,17 +2252,17 @@
       <c r="B83">
         <v>6</v>
       </c>
-      <c r="C83" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D83" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E83" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C83">
+        <f t="shared" si="4"/>
+        <v>1567.981743926998</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="5"/>
+        <v>583</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="6"/>
+        <v>-1.2504338073770214</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2274,17 +2272,17 @@
       <c r="B84">
         <v>6</v>
       </c>
-      <c r="C84" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D84" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E84" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C84">
+        <f t="shared" si="4"/>
+        <v>1661.2187903197814</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="5"/>
+        <v>617</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="6"/>
+        <v>0.47049930415641938</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2294,17 +2292,17 @@
       <c r="B85">
         <v>6</v>
       </c>
-      <c r="C85" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D85" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E85" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C85">
+        <f t="shared" si="4"/>
+        <v>1760.0000000000009</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="5"/>
+        <v>654</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="6"/>
+        <v>-0.33935546874909051</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2314,17 +2312,17 @@
       <c r="B86">
         <v>6</v>
       </c>
-      <c r="C86" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D86" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E86" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C86">
+        <f t="shared" si="4"/>
+        <v>1864.6550460723606</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="5"/>
+        <v>693</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="6"/>
+        <v>-0.65867463076438071</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2334,17 +2332,17 @@
       <c r="B87">
         <v>6</v>
       </c>
-      <c r="C87" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D87" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E87" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C87">
+        <f t="shared" si="4"/>
+        <v>1975.5332050244976</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="5"/>
+        <v>734</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="6"/>
+        <v>-0.13818169425235283</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2354,17 +2352,17 @@
       <c r="B88">
         <v>7</v>
       </c>
-      <c r="C88" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D88" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E88" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C88">
+        <f t="shared" si="4"/>
+        <v>2093.0045224047904</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="5"/>
+        <v>778</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="6"/>
+        <v>-1.0994815014596497</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2374,17 +2372,17 @@
       <c r="B89">
         <v>7</v>
       </c>
-      <c r="C89" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D89" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E89" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C89">
+        <f t="shared" si="4"/>
+        <v>2217.4610478149784</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="5"/>
+        <v>824</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="6"/>
+        <v>-0.45887406002157149</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2394,17 +2392,17 @@
       <c r="B90">
         <v>7</v>
       </c>
-      <c r="C90" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D90" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E90" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C90">
+        <f t="shared" si="4"/>
+        <v>2349.3181433392624</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="5"/>
+        <v>873</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="6"/>
+        <v>-0.49264767636259421</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2414,17 +2412,17 @@
       <c r="B91">
         <v>7</v>
       </c>
-      <c r="C91" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D91" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E91" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C91">
+        <f t="shared" si="4"/>
+        <v>2489.0158697766497</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="5"/>
+        <v>925</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="6"/>
+        <v>-0.76074155147534839</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2434,17 +2432,17 @@
       <c r="B92">
         <v>7</v>
       </c>
-      <c r="C92" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D92" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E92" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C92">
+        <f t="shared" si="4"/>
+        <v>2637.0204553029621</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="5"/>
+        <v>980</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="6"/>
+        <v>-0.79692750953790892</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2454,17 +2452,17 @@
       <c r="B93">
         <v>7</v>
       </c>
-      <c r="C93" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D93" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E93" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C93">
+        <f t="shared" si="4"/>
+        <v>2793.8258514640338</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="5"/>
+        <v>1038</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="6"/>
+        <v>-0.1072540047161965</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2474,17 +2472,17 @@
       <c r="B94">
         <v>7</v>
       </c>
-      <c r="C94" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D94" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E94" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C94">
+        <f t="shared" si="4"/>
+        <v>2959.9553816930784</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="5"/>
+        <v>1100</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="6"/>
+        <v>-0.86004799442162039</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2494,17 +2492,17 @@
       <c r="B95">
         <v>7</v>
       </c>
-      <c r="C95" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D95" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E95" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C95">
+        <f t="shared" si="4"/>
+        <v>3135.9634878539978</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="5"/>
+        <v>1165</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="6"/>
+        <v>0.19078277587277626</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2514,17 +2512,17 @@
       <c r="B96">
         <v>7</v>
       </c>
-      <c r="C96" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D96" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E96" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C96">
+        <f t="shared" si="4"/>
+        <v>3322.4375806395647</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="5"/>
+        <v>1234</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="6"/>
+        <v>0.94099860831465776</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2534,17 +2532,17 @@
       <c r="B97">
         <v>7</v>
       </c>
-      <c r="C97" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D97" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E97" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C97">
+        <f t="shared" si="4"/>
+        <v>3520.0000000000041</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="5"/>
+        <v>1308</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="6"/>
+        <v>-0.67871093749590727</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2554,17 +2552,17 @@
       <c r="B98">
         <v>7</v>
       </c>
-      <c r="C98" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D98" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E98" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C98">
+        <f t="shared" si="4"/>
+        <v>3729.310092144724</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="5"/>
+        <v>1386</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="6"/>
+        <v>-1.3173492615260329</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2574,17 +2572,17 @@
       <c r="B99">
         <v>7</v>
       </c>
-      <c r="C99" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D99" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E99" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C99">
+        <f t="shared" si="4"/>
+        <v>3951.066410048998</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="5"/>
+        <v>1468</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="6"/>
+        <v>-0.27636338850197717</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2594,17 +2592,17 @@
       <c r="B100">
         <v>8</v>
       </c>
-      <c r="C100" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D100" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E100" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C100">
+        <f t="shared" si="4"/>
+        <v>4186.0090448095834</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="5"/>
+        <v>1555</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="6"/>
+        <v>0.49268738770842901</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2614,17 +2612,17 @@
       <c r="B101">
         <v>8</v>
       </c>
-      <c r="C101" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D101" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E101" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C101">
+        <f t="shared" si="4"/>
+        <v>4434.9220956299596</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="5"/>
+        <v>1648</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="6"/>
+        <v>-0.91774812004041451</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2634,17 +2632,17 @@
       <c r="B102">
         <v>8</v>
       </c>
-      <c r="C102" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D102" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E102" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C102">
+        <f t="shared" si="4"/>
+        <v>4698.6362866785275</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="5"/>
+        <v>1746</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="6"/>
+        <v>-0.98529535272245994</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2654,17 +2652,17 @@
       <c r="B103">
         <v>8</v>
       </c>
-      <c r="C103" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D103" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E103" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C103">
+        <f t="shared" si="4"/>
+        <v>4978.031739553302</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="5"/>
+        <v>1849</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="6"/>
+        <v>1.1701672876770317</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2674,17 +2672,17 @@
       <c r="B104">
         <v>8</v>
       </c>
-      <c r="C104" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D104" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E104" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C104">
+        <f t="shared" si="4"/>
+        <v>5274.0409106059269</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="5"/>
+        <v>1959</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="6"/>
+        <v>1.0977953715519106</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2694,17 +2692,17 @@
       <c r="B105">
         <v>8</v>
       </c>
-      <c r="C105" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D105" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E105" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C105">
+        <f t="shared" si="4"/>
+        <v>5587.6517029280712</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="5"/>
+        <v>2076</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="6"/>
+        <v>-0.21450800942875503</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2714,17 +2712,17 @@
       <c r="B106">
         <v>8</v>
       </c>
-      <c r="C106" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D106" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E106" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C106">
+        <f t="shared" si="4"/>
+        <v>5919.9107633861604</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="5"/>
+        <v>2199</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="6"/>
+        <v>0.9715544017853972</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2734,17 +2732,17 @@
       <c r="B107">
         <v>8</v>
       </c>
-      <c r="C107" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D107" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E107" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C107">
+        <f t="shared" si="4"/>
+        <v>6271.9269757079992</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="5"/>
+        <v>2330</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="6"/>
+        <v>0.38156555174919049</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2754,17 +2752,17 @@
       <c r="B108">
         <v>8</v>
       </c>
-      <c r="C108" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D108" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E108" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C108">
+        <f t="shared" si="4"/>
+        <v>6644.8751612791339</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="5"/>
+        <v>2469</v>
+      </c>
+      <c r="E108">
+        <f t="shared" si="6"/>
+        <v>-0.80965317399113701</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2774,17 +2772,17 @@
       <c r="B109">
         <v>8</v>
       </c>
-      <c r="C109" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D109" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E109" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C109">
+        <f t="shared" si="4"/>
+        <v>7040.0000000000127</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="5"/>
+        <v>2615</v>
+      </c>
+      <c r="E109">
+        <f t="shared" si="6"/>
+        <v>1.3342285156377329</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -2794,17 +2792,17 @@
       <c r="B110">
         <v>8</v>
       </c>
-      <c r="C110" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D110" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E110" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C110">
+        <f t="shared" si="4"/>
+        <v>7458.6201842894525</v>
+      </c>
+      <c r="D110">
+        <f t="shared" si="5"/>
+        <v>2771</v>
+      </c>
+      <c r="E110">
+        <f t="shared" si="6"/>
+        <v>5.6951867577481607E-2</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -2814,17 +2812,17 @@
       <c r="B111">
         <v>8</v>
       </c>
-      <c r="C111" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D111" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E111" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C111">
+        <f t="shared" si="4"/>
+        <v>7902.1328200980006</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="5"/>
+        <v>2936</v>
+      </c>
+      <c r="E111">
+        <f t="shared" si="6"/>
+        <v>-0.55272677699940687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct implementation of HPS on tuner_mul Quite some consistent results TODO: - Generalize reference pitch A4 (Assumes 440Hz) - Generalize temperament (Assumes equal temperament) - Include a "index" to "note name" mapper - Derive frequency error estimate - Establish relationships between FFT-size and Sampling Rate
</commit_message>
<xml_diff>
--- a/excel/tuner.xlsx
+++ b/excel/tuner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfredo.CELPLANUS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\SimpleTuner\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B573A9A8-F1E6-474E-B646-0D738B72EAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644212CD-15AD-4AC7-8933-0EBC737ECC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5E2A74D-75EF-4F4E-9939-B924DF3501C3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="35">
   <si>
     <t>A4 Pitch</t>
   </si>
@@ -116,6 +116,30 @@
   </si>
   <si>
     <t>F Err</t>
+  </si>
+  <si>
+    <t>27.5" scale</t>
+  </si>
+  <si>
+    <t>Seed Sago Kotetsu/Makoto Sakamura signature 30" scale not accounted (odd ball)</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>stdev</t>
+  </si>
+  <si>
+    <t>freq error</t>
+  </si>
+  <si>
+    <t>Hz</t>
   </si>
 </sst>
 </file>
@@ -145,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +199,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -200,14 +230,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
@@ -218,8 +249,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="20% - Accent2" xfId="5" builtinId="34"/>
     <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="3" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="4" builtinId="52"/>
@@ -547,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F5B76F-3602-47EF-B36D-B2F7C7714F2D}">
-  <dimension ref="A1:T111"/>
+  <dimension ref="A1:R111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+      <selection activeCell="L5" sqref="L5:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +592,7 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -588,43 +622,27 @@
         <v>18</v>
       </c>
       <c r="K1">
-        <f>2^14</f>
-        <v>16384</v>
+        <f>2^16</f>
+        <v>65536</v>
       </c>
       <c r="M1" t="s">
         <v>19</v>
       </c>
       <c r="N1">
         <f>H1/K1</f>
-        <v>2.691650390625</v>
+        <v>0.67291259765625</v>
       </c>
       <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1">
-        <f>MIN(E4:E111)</f>
-        <v>-1.3173492615260329</v>
-      </c>
-      <c r="R1">
-        <f>MAX(E4:E111)</f>
-        <v>1.3342285156377329</v>
-      </c>
-      <c r="S1">
-        <f>AVERAGE(E4:E111)</f>
-        <v>3.343558368322154E-2</v>
-      </c>
-      <c r="T1">
-        <f>STDEV(E4:E111)</f>
-        <v>0.79945573399802961</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H2">
         <f>K1/H1</f>
-        <v>0.37151927437641724</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+        <v>1.486077097505669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -641,7 +659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -654,14 +672,17 @@
       </c>
       <c r="D4">
         <f>ROUND(C4/$N$1,0)</f>
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <f>C4-D4*$N$1</f>
         <v>0.20169548753737132</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -674,11 +695,21 @@
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D68" si="1">ROUND(C5/$N$1,0)</f>
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5:E14" si="2">C5-D5*$N$1</f>
-        <v>1.1740120923044621</v>
+        <v>-0.17181310300803787</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5">
+        <f>MIN(E4:E111)</f>
+        <v>-0.32933731538230404</v>
+      </c>
+      <c r="L5" t="s">
+        <v>34</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>2</v>
@@ -687,7 +718,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -700,11 +731,21 @@
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>-0.48750473953707285</v>
+        <v>0.18540785811917715</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6">
+        <f>MAX(E4:E111)</f>
+        <v>0.33355712890715949</v>
+      </c>
+      <c r="L6" t="s">
+        <v>34</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>7</v>
@@ -713,7 +754,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -726,11 +767,21 @@
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>0.6038837482550079</v>
+        <v>-6.9028849401242098E-2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7">
+        <f>AVERAGE(E4:E111)</f>
+        <v>-1.0179121720424296E-2</v>
+      </c>
+      <c r="L7" t="s">
+        <v>34</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>12</v>
@@ -739,7 +790,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -752,11 +803,21 @@
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>-0.93148081794567972</v>
+        <v>-0.25856822028942972</v>
+      </c>
+      <c r="J8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8">
+        <f>STDEV(E4:E111)</f>
+        <v>0.20043431293807157</v>
+      </c>
+      <c r="L8" t="s">
+        <v>34</v>
       </c>
       <c r="Q8" s="4" t="s">
         <v>5</v>
@@ -765,7 +826,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -778,14 +839,20 @@
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
         <v>0.29356133956268948</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Q9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -798,14 +865,17 @@
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>-1.1002020961479069</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0.24562309916459313</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -818,14 +888,14 @@
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
         <v>0.27486123323427236</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -838,14 +908,14 @@
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>-0.95996030750348993</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+        <v>-0.28704770984723993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -858,14 +928,14 @@
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>0.58349609374993605</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+        <v>-8.9416503906313949E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -878,14 +948,14 @@
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>-0.47291920199444704</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0.19999339566180296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -898,14 +968,14 @@
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="E15">
         <f t="shared" ref="E15:E78" si="3">C15-D15*$N$1</f>
-        <v>1.2595520316326869</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+        <v>-8.6273163679813081E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -918,11 +988,11 @@
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="E16">
         <f t="shared" si="3"/>
-        <v>0.40339097507475685</v>
+        <v>-0.26952162258149315</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -938,11 +1008,11 @@
       </c>
       <c r="D17" s="6">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="E17" s="6">
         <f t="shared" si="3"/>
-        <v>-0.34362620601606153</v>
+        <v>0.32928639164018847</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -958,11 +1028,11 @@
       </c>
       <c r="D18" s="6">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="E18" s="6">
         <f t="shared" si="3"/>
-        <v>-0.97500947907413149</v>
+        <v>-0.30209688141788149</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -978,11 +1048,11 @@
       </c>
       <c r="D19" s="6">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E19" s="6">
         <f t="shared" si="3"/>
-        <v>1.2077674965100371</v>
+        <v>-0.13805769880246288</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -998,11 +1068,11 @@
       </c>
       <c r="D20" s="6">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="E20" s="6">
         <f t="shared" si="3"/>
-        <v>0.82868875473366188</v>
+        <v>0.15577615707741188</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1018,11 +1088,11 @@
       </c>
       <c r="D21" s="6">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="E21" s="6">
         <f t="shared" si="3"/>
-        <v>0.58712267912540028</v>
+        <v>-8.5789918530849718E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1038,11 +1108,11 @@
       </c>
       <c r="D22" s="6">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="E22" s="6">
         <f t="shared" si="3"/>
-        <v>0.49124619832921468</v>
+        <v>-0.18166639932703532</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1058,11 +1128,11 @@
       </c>
       <c r="D23" s="6">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="E23" s="6">
         <f t="shared" si="3"/>
-        <v>0.54972246646857315</v>
+        <v>-0.12319013118767685</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1078,11 +1148,11 @@
       </c>
       <c r="D24" s="6">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="E24" s="6">
         <f t="shared" si="3"/>
-        <v>0.77172977561804856</v>
+        <v>9.8817177961798564E-2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1098,11 +1168,11 @@
       </c>
       <c r="D25" s="6">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="E25" s="6">
         <f t="shared" si="3"/>
-        <v>1.1669921874999005</v>
+        <v>-0.17883300781259948</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1118,11 +1188,11 @@
       </c>
       <c r="D26" s="6">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="E26" s="6">
         <f t="shared" si="3"/>
-        <v>-0.94583840398886565</v>
+        <v>-0.27292580633261565</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1138,7 +1208,7 @@
       </c>
       <c r="D27" s="6">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="E27" s="6">
         <f t="shared" si="3"/>
@@ -1158,11 +1228,11 @@
       </c>
       <c r="D28" s="6">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>97</v>
       </c>
       <c r="E28" s="6">
         <f t="shared" si="3"/>
-        <v>0.80678195014954213</v>
+        <v>0.13386935249329213</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1178,11 +1248,11 @@
       </c>
       <c r="D29" s="6">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>103</v>
       </c>
       <c r="E29" s="6">
         <f t="shared" si="3"/>
-        <v>-0.68725241203209464</v>
+        <v>-1.4339814375844639E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1198,11 +1268,11 @@
       </c>
       <c r="D30" s="6">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="E30" s="6">
         <f t="shared" si="3"/>
-        <v>0.74163143247676544</v>
+        <v>6.871883482051544E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1218,7 +1288,7 @@
       </c>
       <c r="D31" s="6">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>116</v>
       </c>
       <c r="E31" s="6">
         <f t="shared" si="3"/>
@@ -1238,11 +1308,11 @@
       </c>
       <c r="D32" s="6">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>122</v>
       </c>
       <c r="E32" s="6">
         <f t="shared" si="3"/>
-        <v>-1.0342728811576478</v>
+        <v>0.31155231415485218</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1258,11 +1328,11 @@
       </c>
       <c r="D33" s="6">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="E33" s="6">
         <f t="shared" si="3"/>
-        <v>1.1742453582508432</v>
+        <v>-0.1715798370616568</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1278,11 +1348,11 @@
       </c>
       <c r="D34" s="6">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>137</v>
       </c>
       <c r="E34" s="6">
         <f t="shared" si="3"/>
-        <v>0.98249239665847199</v>
+        <v>0.30957979900222199</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1298,11 +1368,11 @@
       </c>
       <c r="D35" s="6">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>146</v>
       </c>
       <c r="E35" s="6">
         <f t="shared" si="3"/>
-        <v>1.0994449329371889</v>
+        <v>-0.24638026237531108</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1318,11 +1388,11 @@
       </c>
       <c r="D36" s="6">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>154</v>
       </c>
       <c r="E36" s="6">
         <f t="shared" si="3"/>
-        <v>-1.148190839388846</v>
+        <v>0.19763435592365397</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1338,11 +1408,11 @@
       </c>
       <c r="D37" s="6">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>163</v>
       </c>
       <c r="E37" s="6">
         <f t="shared" si="3"/>
-        <v>-0.3576660156251279</v>
+        <v>0.3152465820311221</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1358,11 +1428,11 @@
       </c>
       <c r="D38" s="6">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="E38" s="6">
         <f t="shared" si="3"/>
-        <v>0.79997358264735396</v>
+        <v>0.12706098499110396</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1378,11 +1448,11 @@
       </c>
       <c r="D39" s="6">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>183</v>
       </c>
       <c r="E39" s="6">
         <f t="shared" si="3"/>
-        <v>-0.345092654719096</v>
+        <v>0.327819942937154</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1398,11 +1468,11 @@
       </c>
       <c r="D40" s="6">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>194</v>
       </c>
       <c r="E40" s="6">
         <f t="shared" si="3"/>
-        <v>-1.0780864903258021</v>
+        <v>0.26773870498669794</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1418,11 +1488,11 @@
       </c>
       <c r="D41" s="6">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>206</v>
       </c>
       <c r="E41" s="6">
         <f t="shared" si="3"/>
-        <v>1.3171455665609244</v>
+        <v>-2.8679628751575592E-2</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1438,11 +1508,11 @@
       </c>
       <c r="D42" s="6">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>218</v>
       </c>
       <c r="E42" s="6">
         <f t="shared" si="3"/>
-        <v>-1.2083875256713554</v>
+        <v>0.13743766964114457</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1458,11 +1528,11 @@
       </c>
       <c r="D43" s="6">
         <f t="shared" si="1"/>
-        <v>58</v>
+        <v>231</v>
       </c>
       <c r="E43" s="6">
         <f t="shared" si="3"/>
-        <v>-0.55223079520968099</v>
+        <v>0.12068180244656901</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1478,11 +1548,11 @@
       </c>
       <c r="D44" s="6">
         <f t="shared" si="1"/>
-        <v>61</v>
+        <v>245</v>
       </c>
       <c r="E44" s="6">
         <f t="shared" si="3"/>
-        <v>0.62310462830981805</v>
+        <v>-4.9807969346431946E-2</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1498,11 +1568,11 @@
       </c>
       <c r="D45" s="6">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>259</v>
       </c>
       <c r="E45" s="6">
         <f t="shared" si="3"/>
-        <v>-0.34315967412319992</v>
+        <v>0.32975292353305008</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1518,11 +1588,11 @@
       </c>
       <c r="D46" s="6">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>275</v>
       </c>
       <c r="E46" s="6">
         <f t="shared" si="3"/>
-        <v>-0.72666559730794233</v>
+        <v>-5.3752999651692335E-2</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1538,11 +1608,11 @@
       </c>
       <c r="D47" s="6">
         <f t="shared" si="1"/>
-        <v>73</v>
+        <v>291</v>
       </c>
       <c r="E47" s="6">
         <f t="shared" si="3"/>
-        <v>-0.49276052475050847</v>
+        <v>0.18015207290574153</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1558,11 +1628,11 @@
       </c>
       <c r="D48" s="6">
         <f t="shared" si="1"/>
-        <v>77</v>
+        <v>309</v>
       </c>
       <c r="E48" s="6">
         <f t="shared" si="3"/>
-        <v>0.39526871184742163</v>
+        <v>-0.27764388580882837</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1578,11 +1648,11 @@
       </c>
       <c r="D49" s="6">
         <f t="shared" si="1"/>
-        <v>82</v>
+        <v>327</v>
       </c>
       <c r="E49" s="6">
         <f t="shared" si="3"/>
-        <v>-0.71533203125014211</v>
+        <v>-4.2419433593892109E-2</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1598,11 +1668,11 @@
       </c>
       <c r="D50" s="6">
         <f t="shared" si="1"/>
-        <v>87</v>
+        <v>346</v>
       </c>
       <c r="E50" s="6">
         <f t="shared" si="3"/>
-        <v>-1.0917032253301784</v>
+        <v>0.25412196998232162</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1618,11 +1688,11 @@
       </c>
       <c r="D51" s="6">
         <f t="shared" si="1"/>
-        <v>92</v>
+        <v>367</v>
       </c>
       <c r="E51" s="6">
         <f t="shared" si="3"/>
-        <v>-0.69018530943807832</v>
+        <v>-1.727271178182832E-2</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1638,11 +1708,11 @@
       </c>
       <c r="D52" s="6">
         <f t="shared" si="1"/>
-        <v>97</v>
+        <v>389</v>
       </c>
       <c r="E52" s="6">
         <f t="shared" si="3"/>
-        <v>0.53547740997350957</v>
+        <v>-0.13743518768274043</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1658,7 +1728,7 @@
       </c>
       <c r="D53" s="6">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>412</v>
       </c>
       <c r="E53" s="6">
         <f t="shared" si="3"/>
@@ -1678,7 +1748,7 @@
       </c>
       <c r="D54" s="6">
         <f t="shared" si="1"/>
-        <v>109</v>
+        <v>436</v>
       </c>
       <c r="E54" s="6">
         <f t="shared" si="3"/>
@@ -1698,11 +1768,11 @@
       </c>
       <c r="D55" s="6">
         <f t="shared" si="1"/>
-        <v>116</v>
+        <v>462</v>
       </c>
       <c r="E55" s="6">
         <f t="shared" si="3"/>
-        <v>-1.1044615904191915</v>
+        <v>0.24136360489330855</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1718,11 +1788,11 @@
       </c>
       <c r="D56" s="6">
         <f t="shared" si="1"/>
-        <v>122</v>
+        <v>490</v>
       </c>
       <c r="E56" s="6">
         <f t="shared" si="3"/>
-        <v>1.2462092566198635</v>
+        <v>-9.9615938692636519E-2</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1738,11 +1808,11 @@
       </c>
       <c r="D57" s="6">
         <f t="shared" si="1"/>
-        <v>130</v>
+        <v>519</v>
       </c>
       <c r="E57" s="6">
         <f t="shared" si="3"/>
-        <v>-0.68631934824617247</v>
+        <v>-1.3406750589922467E-2</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1758,11 +1828,11 @@
       </c>
       <c r="D58" s="6">
         <f t="shared" si="1"/>
-        <v>137</v>
+        <v>550</v>
       </c>
       <c r="E58" s="6">
         <f t="shared" si="3"/>
-        <v>1.2383191960093427</v>
+        <v>-0.1075059993031573</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1778,11 +1848,11 @@
       </c>
       <c r="D59" s="6">
         <f t="shared" si="1"/>
-        <v>146</v>
+        <v>583</v>
       </c>
       <c r="E59" s="6">
         <f t="shared" si="3"/>
-        <v>-0.98552104950073272</v>
+        <v>-0.31260845184448272</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1798,11 +1868,11 @@
       </c>
       <c r="D60" s="6">
         <f t="shared" si="1"/>
-        <v>154</v>
+        <v>617</v>
       </c>
       <c r="E60" s="6">
         <f t="shared" si="3"/>
-        <v>0.79053742369512747</v>
+        <v>0.11762482603887747</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1818,11 +1888,11 @@
       </c>
       <c r="D61" s="6">
         <f t="shared" si="1"/>
-        <v>163</v>
+        <v>654</v>
       </c>
       <c r="E61" s="6">
         <f t="shared" si="3"/>
-        <v>1.260986328125</v>
+        <v>-8.48388671875E-2</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1838,11 +1908,11 @@
       </c>
       <c r="D62" s="6">
         <f t="shared" si="1"/>
-        <v>173</v>
+        <v>693</v>
       </c>
       <c r="E62" s="6">
         <f t="shared" si="3"/>
-        <v>0.50824393996492745</v>
+        <v>-0.16466865769132255</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1858,11 +1928,11 @@
       </c>
       <c r="D63" s="6">
         <f t="shared" si="1"/>
-        <v>183</v>
+        <v>734</v>
       </c>
       <c r="E63" s="6">
         <f t="shared" si="3"/>
-        <v>1.3112797717491276</v>
+        <v>-3.4545423563372424E-2</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1878,11 +1948,11 @@
       </c>
       <c r="D64" s="6">
         <f t="shared" si="1"/>
-        <v>194</v>
+        <v>778</v>
       </c>
       <c r="E64" s="6">
         <f t="shared" si="3"/>
-        <v>1.0709548199473602</v>
+        <v>-0.27487037536513981</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1898,7 +1968,7 @@
       </c>
       <c r="D65" s="6">
         <f t="shared" si="1"/>
-        <v>206</v>
+        <v>824</v>
       </c>
       <c r="E65" s="6">
         <f t="shared" si="3"/>
@@ -1918,11 +1988,11 @@
       </c>
       <c r="D66" s="6">
         <f t="shared" si="1"/>
-        <v>218</v>
+        <v>873</v>
       </c>
       <c r="E66" s="6">
         <f t="shared" si="3"/>
-        <v>0.54975067856526039</v>
+        <v>-0.12316191909098961</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1938,11 +2008,11 @@
       </c>
       <c r="D67" s="6">
         <f t="shared" si="1"/>
-        <v>231</v>
+        <v>925</v>
       </c>
       <c r="E67" s="6">
         <f t="shared" si="3"/>
-        <v>0.48272720978695816</v>
+        <v>-0.19018538786929184</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1958,7 +2028,7 @@
       </c>
       <c r="D68" s="6">
         <f t="shared" si="1"/>
-        <v>245</v>
+        <v>980</v>
       </c>
       <c r="E68" s="6">
         <f t="shared" si="3"/>
@@ -1978,11 +2048,11 @@
       </c>
       <c r="D69" s="6">
         <f t="shared" ref="D69:D111" si="5">ROUND(C69/$N$1,0)</f>
-        <v>259</v>
+        <v>1038</v>
       </c>
       <c r="E69" s="6">
         <f t="shared" si="3"/>
-        <v>1.3190116941329961</v>
+        <v>-2.6813501179503874E-2</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1998,7 +2068,7 @@
       </c>
       <c r="D70" s="6">
         <f t="shared" si="5"/>
-        <v>275</v>
+        <v>1100</v>
       </c>
       <c r="E70" s="6">
         <f t="shared" si="3"/>
@@ -2018,11 +2088,11 @@
       </c>
       <c r="D71" s="6">
         <f t="shared" si="5"/>
-        <v>291</v>
+        <v>1165</v>
       </c>
       <c r="E71" s="6">
         <f t="shared" si="3"/>
-        <v>0.72060829162387563</v>
+        <v>4.769569396762563E-2</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2038,11 +2108,11 @@
       </c>
       <c r="D72" s="6">
         <f t="shared" si="5"/>
-        <v>309</v>
+        <v>1234</v>
       </c>
       <c r="E72" s="6">
         <f t="shared" si="3"/>
-        <v>-1.110575543234404</v>
+        <v>0.23524965207809601</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2058,7 +2128,7 @@
       </c>
       <c r="D73" s="6">
         <f t="shared" si="5"/>
-        <v>327</v>
+        <v>1308</v>
       </c>
       <c r="E73" s="6">
         <f t="shared" si="3"/>
@@ -2078,11 +2148,11 @@
       </c>
       <c r="D74" s="6">
         <f t="shared" si="5"/>
-        <v>346</v>
+        <v>1386</v>
       </c>
       <c r="E74" s="6">
         <f t="shared" si="3"/>
-        <v>1.016487879930196</v>
+        <v>-0.32933731538230404</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2098,7 +2168,7 @@
       </c>
       <c r="D75" s="6">
         <f t="shared" si="5"/>
-        <v>367</v>
+        <v>1468</v>
       </c>
       <c r="E75" s="6">
         <f t="shared" si="3"/>
@@ -2118,11 +2188,11 @@
       </c>
       <c r="D76" s="6">
         <f t="shared" si="5"/>
-        <v>389</v>
+        <v>1555</v>
       </c>
       <c r="E76" s="6">
         <f t="shared" si="3"/>
-        <v>-0.54974075073005224</v>
+        <v>0.12317184692619776</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2138,7 +2208,7 @@
       </c>
       <c r="D77" s="6">
         <f t="shared" si="5"/>
-        <v>412</v>
+        <v>1648</v>
       </c>
       <c r="E77" s="6">
         <f t="shared" si="3"/>
@@ -2158,11 +2228,11 @@
       </c>
       <c r="D78" s="6">
         <f t="shared" si="5"/>
-        <v>436</v>
+        <v>1746</v>
       </c>
       <c r="E78" s="6">
         <f t="shared" si="3"/>
-        <v>1.0995013571307481</v>
+        <v>-0.24632383818175185</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2178,11 +2248,11 @@
       </c>
       <c r="D79" s="6">
         <f t="shared" si="5"/>
-        <v>462</v>
+        <v>1849</v>
       </c>
       <c r="E79" s="6">
         <f t="shared" ref="E79:E111" si="6">C79-D79*$N$1</f>
-        <v>0.96545441957414369</v>
+        <v>0.29254182191789369</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2198,71 +2268,71 @@
       </c>
       <c r="D80" s="6">
         <f t="shared" si="5"/>
-        <v>490</v>
+        <v>1959</v>
       </c>
       <c r="E80" s="6">
         <f t="shared" si="6"/>
-        <v>-0.39846375476963658</v>
+        <v>0.27444884288661342</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="A81" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="11">
         <v>6</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="6">
         <f t="shared" si="4"/>
         <v>1396.9129257320162</v>
       </c>
-      <c r="D81">
-        <f t="shared" si="5"/>
-        <v>519</v>
-      </c>
-      <c r="E81">
+      <c r="D81" s="6">
+        <f t="shared" si="5"/>
+        <v>2076</v>
+      </c>
+      <c r="E81" s="6">
         <f t="shared" si="6"/>
         <v>-5.3627002358780373E-2</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="A82" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="11">
         <v>6</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="6">
         <f t="shared" si="4"/>
         <v>1479.9776908465383</v>
       </c>
-      <c r="D82">
-        <f t="shared" si="5"/>
-        <v>550</v>
-      </c>
-      <c r="E82">
-        <f t="shared" si="6"/>
-        <v>-0.43002399721171969</v>
+      <c r="D82" s="6">
+        <f t="shared" si="5"/>
+        <v>2199</v>
+      </c>
+      <c r="E82" s="6">
+        <f t="shared" si="6"/>
+        <v>0.24288860044453031</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="A83" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="11">
         <v>6</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="6">
         <f t="shared" si="4"/>
         <v>1567.981743926998</v>
       </c>
-      <c r="D83">
-        <f t="shared" si="5"/>
-        <v>583</v>
-      </c>
-      <c r="E83">
-        <f t="shared" si="6"/>
-        <v>-1.2504338073770214</v>
+      <c r="D83" s="6">
+        <f t="shared" si="5"/>
+        <v>2330</v>
+      </c>
+      <c r="E83" s="6">
+        <f t="shared" si="6"/>
+        <v>9.5391387935478633E-2</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2278,11 +2348,11 @@
       </c>
       <c r="D84">
         <f t="shared" si="5"/>
-        <v>617</v>
+        <v>2469</v>
       </c>
       <c r="E84">
         <f t="shared" si="6"/>
-        <v>0.47049930415641938</v>
+        <v>-0.20241329349983062</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2298,11 +2368,11 @@
       </c>
       <c r="D85">
         <f t="shared" si="5"/>
-        <v>654</v>
+        <v>2615</v>
       </c>
       <c r="E85">
         <f t="shared" si="6"/>
-        <v>-0.33935546874909051</v>
+        <v>0.33355712890715949</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2318,11 +2388,11 @@
       </c>
       <c r="D86">
         <f t="shared" si="5"/>
-        <v>693</v>
+        <v>2771</v>
       </c>
       <c r="E86">
         <f t="shared" si="6"/>
-        <v>-0.65867463076438071</v>
+        <v>1.4237966891869291E-2</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2338,7 +2408,7 @@
       </c>
       <c r="D87">
         <f t="shared" si="5"/>
-        <v>734</v>
+        <v>2936</v>
       </c>
       <c r="E87">
         <f t="shared" si="6"/>
@@ -2358,11 +2428,11 @@
       </c>
       <c r="D88">
         <f t="shared" si="5"/>
-        <v>778</v>
+        <v>3110</v>
       </c>
       <c r="E88">
         <f t="shared" si="6"/>
-        <v>-1.0994815014596497</v>
+        <v>0.24634369385285027</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2378,11 +2448,11 @@
       </c>
       <c r="D89">
         <f t="shared" si="5"/>
-        <v>824</v>
+        <v>3295</v>
       </c>
       <c r="E89">
         <f t="shared" si="6"/>
-        <v>-0.45887406002157149</v>
+        <v>0.21403853763467851</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2398,11 +2468,11 @@
       </c>
       <c r="D90">
         <f t="shared" si="5"/>
-        <v>873</v>
+        <v>3491</v>
       </c>
       <c r="E90">
         <f t="shared" si="6"/>
-        <v>-0.49264767636259421</v>
+        <v>0.18026492129365579</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2418,11 +2488,11 @@
       </c>
       <c r="D91">
         <f t="shared" si="5"/>
-        <v>925</v>
+        <v>3699</v>
       </c>
       <c r="E91">
         <f t="shared" si="6"/>
-        <v>-0.76074155147534839</v>
+        <v>-8.7828953819098388E-2</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2438,11 +2508,11 @@
       </c>
       <c r="D92">
         <f t="shared" si="5"/>
-        <v>980</v>
+        <v>3919</v>
       </c>
       <c r="E92">
         <f t="shared" si="6"/>
-        <v>-0.79692750953790892</v>
+        <v>-0.12401491188165892</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2458,7 +2528,7 @@
       </c>
       <c r="D93">
         <f t="shared" si="5"/>
-        <v>1038</v>
+        <v>4152</v>
       </c>
       <c r="E93">
         <f t="shared" si="6"/>
@@ -2478,11 +2548,11 @@
       </c>
       <c r="D94">
         <f t="shared" si="5"/>
-        <v>1100</v>
+        <v>4399</v>
       </c>
       <c r="E94">
         <f t="shared" si="6"/>
-        <v>-0.86004799442162039</v>
+        <v>-0.18713539676537039</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2498,7 +2568,7 @@
       </c>
       <c r="D95">
         <f t="shared" si="5"/>
-        <v>1165</v>
+        <v>4660</v>
       </c>
       <c r="E95">
         <f t="shared" si="6"/>
@@ -2518,11 +2588,11 @@
       </c>
       <c r="D96">
         <f t="shared" si="5"/>
-        <v>1234</v>
+        <v>4937</v>
       </c>
       <c r="E96">
         <f t="shared" si="6"/>
-        <v>0.94099860831465776</v>
+        <v>0.26808601065840776</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2538,11 +2608,11 @@
       </c>
       <c r="D97">
         <f t="shared" si="5"/>
-        <v>1308</v>
+        <v>5231</v>
       </c>
       <c r="E97">
         <f t="shared" si="6"/>
-        <v>-0.67871093749590727</v>
+        <v>-5.7983398396572738E-3</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2558,11 +2628,11 @@
       </c>
       <c r="D98">
         <f t="shared" si="5"/>
-        <v>1386</v>
+        <v>5542</v>
       </c>
       <c r="E98">
         <f t="shared" si="6"/>
-        <v>-1.3173492615260329</v>
+        <v>2.8475933786467067E-2</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2578,7 +2648,7 @@
       </c>
       <c r="D99">
         <f t="shared" si="5"/>
-        <v>1468</v>
+        <v>5872</v>
       </c>
       <c r="E99">
         <f t="shared" si="6"/>
@@ -2598,11 +2668,11 @@
       </c>
       <c r="D100">
         <f t="shared" si="5"/>
-        <v>1555</v>
+        <v>6221</v>
       </c>
       <c r="E100">
         <f t="shared" si="6"/>
-        <v>0.49268738770842901</v>
+        <v>-0.18022520994782099</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2618,11 +2688,11 @@
       </c>
       <c r="D101">
         <f t="shared" si="5"/>
-        <v>1648</v>
+        <v>6591</v>
       </c>
       <c r="E101">
         <f t="shared" si="6"/>
-        <v>-0.91774812004041451</v>
+        <v>-0.24483552238416451</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2638,11 +2708,11 @@
       </c>
       <c r="D102">
         <f t="shared" si="5"/>
-        <v>1746</v>
+        <v>6983</v>
       </c>
       <c r="E102">
         <f t="shared" si="6"/>
-        <v>-0.98529535272245994</v>
+        <v>-0.31238275506620994</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2658,11 +2728,11 @@
       </c>
       <c r="D103">
         <f t="shared" si="5"/>
-        <v>1849</v>
+        <v>7398</v>
       </c>
       <c r="E103">
         <f t="shared" si="6"/>
-        <v>1.1701672876770317</v>
+        <v>-0.17565790763546829</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2678,11 +2748,11 @@
       </c>
       <c r="D104">
         <f t="shared" si="5"/>
-        <v>1959</v>
+        <v>7838</v>
       </c>
       <c r="E104">
         <f t="shared" si="6"/>
-        <v>1.0977953715519106</v>
+        <v>-0.24802982376058935</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2698,7 +2768,7 @@
       </c>
       <c r="D105">
         <f t="shared" si="5"/>
-        <v>2076</v>
+        <v>8304</v>
       </c>
       <c r="E105">
         <f t="shared" si="6"/>
@@ -2718,11 +2788,11 @@
       </c>
       <c r="D106">
         <f t="shared" si="5"/>
-        <v>2199</v>
+        <v>8797</v>
       </c>
       <c r="E106">
         <f t="shared" si="6"/>
-        <v>0.9715544017853972</v>
+        <v>0.2986418041291472</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2738,11 +2808,11 @@
       </c>
       <c r="D107">
         <f t="shared" si="5"/>
-        <v>2330</v>
+        <v>9321</v>
       </c>
       <c r="E107">
         <f t="shared" si="6"/>
-        <v>0.38156555174919049</v>
+        <v>-0.29134704590705951</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2758,11 +2828,11 @@
       </c>
       <c r="D108">
         <f t="shared" si="5"/>
-        <v>2469</v>
+        <v>9875</v>
       </c>
       <c r="E108">
         <f t="shared" si="6"/>
-        <v>-0.80965317399113701</v>
+        <v>-0.13674057633488701</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2778,11 +2848,11 @@
       </c>
       <c r="D109">
         <f t="shared" si="5"/>
-        <v>2615</v>
+        <v>10462</v>
       </c>
       <c r="E109">
         <f t="shared" si="6"/>
-        <v>1.3342285156377329</v>
+        <v>-1.1596679674767074E-2</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -2798,7 +2868,7 @@
       </c>
       <c r="D110">
         <f t="shared" si="5"/>
-        <v>2771</v>
+        <v>11084</v>
       </c>
       <c r="E110">
         <f t="shared" si="6"/>
@@ -2818,11 +2888,11 @@
       </c>
       <c r="D111">
         <f t="shared" si="5"/>
-        <v>2936</v>
+        <v>11743</v>
       </c>
       <c r="E111">
         <f t="shared" si="6"/>
-        <v>-0.55272677699940687</v>
+        <v>0.12018582065684313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected a typo on the spreadsheet
</commit_message>
<xml_diff>
--- a/excel/tuner.xlsx
+++ b/excel/tuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\SimpleTuner\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644212CD-15AD-4AC7-8933-0EBC737ECC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511FCF86-9405-4530-BB79-3436860F2C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5E2A74D-75EF-4F4E-9939-B924DF3501C3}"/>
   </bookViews>
@@ -121,9 +121,6 @@
     <t>27.5" scale</t>
   </si>
   <si>
-    <t>Seed Sago Kotetsu/Makoto Sakamura signature 30" scale not accounted (odd ball)</t>
-  </si>
-  <si>
     <t>min</t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>Hz</t>
+  </si>
+  <si>
+    <t>Seed Sago Kotetsu/Makoto Sakamura signature 33" scale not accounted (odd ball)</t>
   </si>
 </sst>
 </file>
@@ -584,7 +584,7 @@
   <dimension ref="A1:R111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:L8"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +679,7 @@
         <v>0.20169548753737132</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -702,14 +702,14 @@
         <v>-0.17181310300803787</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5">
         <f>MIN(E4:E111)</f>
         <v>-0.32933731538230404</v>
       </c>
       <c r="L5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>2</v>
@@ -738,14 +738,14 @@
         <v>0.18540785811917715</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K6">
         <f>MAX(E4:E111)</f>
         <v>0.33355712890715949</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>7</v>
@@ -774,14 +774,14 @@
         <v>-6.9028849401242098E-2</v>
       </c>
       <c r="J7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K7">
         <f>AVERAGE(E4:E111)</f>
         <v>-1.0179121720424296E-2</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>12</v>
@@ -810,14 +810,14 @@
         <v>-0.25856822028942972</v>
       </c>
       <c r="J8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K8">
         <f>STDEV(E4:E111)</f>
         <v>0.20043431293807157</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q8" s="4" t="s">
         <v>5</v>
@@ -872,7 +872,7 @@
         <v>0.24562309916459313</v>
       </c>
       <c r="Q10" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Improvements: 2022/08/11 - Automatically determine the best (tradeoff) prime for the size of FFT   based on the sampling rate.     The tradeoff here is the frequency resolution and FFT complexity.     - Print out a log file with the detected pitch, expected pitch,       error and note name       - Error is not compensated for quantisation error yet       - Reference pitch is now an input parameter
</commit_message>
<xml_diff>
--- a/excel/tuner.xlsx
+++ b/excel/tuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\SimpleTuner\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511FCF86-9405-4530-BB79-3436860F2C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A15EC1-9749-433A-963C-C35656C9F0DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5E2A74D-75EF-4F4E-9939-B924DF3501C3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="36">
   <si>
     <t>A4 Pitch</t>
   </si>
@@ -139,7 +139,10 @@
     <t>Hz</t>
   </si>
   <si>
-    <t>Seed Sago Kotetsu/Makoto Sakamura signature 33" scale not accounted (odd ball)</t>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Seed Sago Kotetsu/Makoto Sakuramura signature 33" scale not accounted (odd ball)</t>
   </si>
 </sst>
 </file>
@@ -622,7 +625,7 @@
         <v>18</v>
       </c>
       <c r="K1">
-        <f>2^16</f>
+        <f>$K$2^(INT(LOG(H1,$K$2))+1)</f>
         <v>65536</v>
       </c>
       <c r="M1" t="s">
@@ -641,6 +644,12 @@
         <f>K1/H1</f>
         <v>1.486077097505669</v>
       </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -872,7 +881,7 @@
         <v>0.24562309916459313</v>
       </c>
       <c r="Q10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>